<commit_message>
idk whats up with this
</commit_message>
<xml_diff>
--- a/www/RPTOOL_WQS_Template.xlsx
+++ b/www/RPTOOL_WQS_Template.xlsx
@@ -2,22 +2,22 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/fisher_adam_epa_gov/Documents/Projects/Clean Water Regulatory Branch/NPDES Section/RPA Tool/RPA app/www/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="89" documentId="8_{D3A1C9D9-45B7-4774-BF38-791F32C01590}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F7A3E27-A87D-42D3-8EEA-A2728993E1CD}"/>
+  <xr:revisionPtr revIDLastSave="95" documentId="8_{D3A1C9D9-45B7-4774-BF38-791F32C01590}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0B8D67E9-35CE-4DAE-95DE-9B6D74AB2C23}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="16663" windowHeight="8863" tabRatio="554" xr2:uid="{0CD2DB0D-7E63-42E8-940B-D4E5BF2F4DC9}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="16663" windowHeight="8863" tabRatio="554" activeTab="1" xr2:uid="{0CD2DB0D-7E63-42E8-940B-D4E5BF2F4DC9}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="2" r:id="rId1"/>
     <sheet name="WQS" sheetId="1" r:id="rId2"/>
     <sheet name="Data Dictionary" sheetId="3" r:id="rId3"/>
     <sheet name="Parameter Domains" sheetId="4" r:id="rId4"/>
-    <sheet name="Unit Dimains" sheetId="5" r:id="rId5"/>
+    <sheet name="Unit Domains" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -31,7 +31,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -92,19 +91,19 @@
     <t>Column Description</t>
   </si>
   <si>
-    <t>Name of the wqs parameter</t>
-  </si>
-  <si>
-    <t>Name of the wqs parameter as reported in ECHO</t>
-  </si>
-  <si>
     <t>Marine water quality standard</t>
   </si>
   <si>
     <t>Freshwater water quality standard</t>
   </si>
   <si>
-    <t>Unit of parameter as reported in ECHO</t>
+    <t>Unit of parameter as reported in ECHO. Restricted to only those listed in the Unit Domains tab.</t>
+  </si>
+  <si>
+    <t>Name of the wqs parameter.</t>
+  </si>
+  <si>
+    <t>Name of the wqs parameter as reported in ECHO. Restricted to only those listed in the Parameter Domains tab</t>
   </si>
 </sst>
 </file>
@@ -459,9 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0A51EBC-9E33-4DCB-B590-CDBA98E7804A}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A2:A8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.45" x14ac:dyDescent="0.5"/>
   <sheetData>
@@ -507,9 +507,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71BFC294-19D0-4914-A04A-9B613DC5C636}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.45" x14ac:dyDescent="0.5"/>
   <cols>
@@ -562,9 +565,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63F4B5E1-A5A9-4E3A-875D-360642914778}">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.45" x14ac:dyDescent="0.5"/>
   <cols>
@@ -585,7 +591,7 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.5">
@@ -593,7 +599,7 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.5">
@@ -601,7 +607,7 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.5">
@@ -609,7 +615,7 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.5">
@@ -617,7 +623,7 @@
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -627,6 +633,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCAEA034-A0D8-493C-B0E9-07EE1EA6265C}">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -639,6 +646,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2A866BC-4362-43B0-820A-EA99E9A0BA40}">
+  <sheetPr codeName="Sheet5"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>